<commit_message>
Retirada de credenciais o arquivo Enviar.xlsx
</commit_message>
<xml_diff>
--- a/Enviar.xlsx
+++ b/Enviar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninin\PycharmProjects\enviar-msg-whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520CBF7C-9802-4154-8804-6A4C3CB241F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AF1C4B-65E5-48F3-80CD-E6DDB9DA8316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{F81C85CE-3BCD-4B33-8C8B-0A39913C8743}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F81C85CE-3BCD-4B33-8C8B-0A39913C8743}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>OI</t>
   </si>
   <si>
-    <t>5579981257925</t>
+    <t>Número de destino</t>
   </si>
 </sst>
 </file>
@@ -86,11 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,17 +407,17 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -440,14 +439,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
   </sheetData>

</xml_diff>